<commit_message>
correction de Feced Offers terminada
</commit_message>
<xml_diff>
--- a/APM files/130228590/120493895 EXPORT RT&RP Cloud Export_Clone.xlsx
+++ b/APM files/130228590/120493895 EXPORT RT&RP Cloud Export_Clone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\github-repositories\core_ota\Expedia Templates\BMC\BMC2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darkesthj/dev/workspace/APM files/130228590/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F60A91-D681-47E9-9478-A4E69D0B0795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCC9CED-44E0-1F4A-8F3B-431F6BE82204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7005" yWindow="5550" windowWidth="24300" windowHeight="14790" xr2:uid="{2547B3A6-92DE-4DC7-BA33-295CE429FBF9}"/>
+    <workbookView xWindow="5180" yWindow="2420" windowWidth="24300" windowHeight="14800" xr2:uid="{2547B3A6-92DE-4DC7-BA33-295CE429FBF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Hotel ID</t>
   </si>
@@ -192,13 +192,16 @@
   </si>
   <si>
     <t>Rate Plan Pricing Model</t>
+  </si>
+  <si>
+    <t> 95545447</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,12 +236,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -255,11 +252,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -267,26 +265,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD5D3D1"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD5D3D1"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD5D3D1"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD5D3D1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -301,7 +284,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,9 +306,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -360,7 +346,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -466,7 +452,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -608,7 +594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -616,64 +602,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C0776E-D31D-4196-98AA-2098101953BE}">
-  <dimension ref="A1:BA48"/>
+  <dimension ref="A1:BA251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="40.5" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="8.5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="20" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="20" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.5" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="18" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,148 +818,1255 @@
       </c>
       <c r="BA1" s="5"/>
     </row>
-    <row r="2" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-    </row>
-    <row r="4" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-    </row>
-    <row r="5" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-    </row>
-    <row r="6" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-    </row>
-    <row r="7" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-    </row>
-    <row r="9" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-    </row>
-    <row r="10" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-    </row>
-    <row r="13" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-    </row>
-    <row r="14" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-    </row>
-    <row r="16" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-    </row>
-    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-    </row>
-    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-    </row>
-    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-    </row>
-    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-    </row>
-    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-    </row>
-    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-    </row>
-    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-    </row>
-    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-    </row>
-    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-    </row>
-    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-    </row>
-    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-    </row>
-    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-    </row>
-    <row r="46" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-    </row>
-    <row r="47" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-    </row>
-    <row r="48" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>17267463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>17268185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>17268291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>17429448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>17475800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>17670891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>17672644</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>17673299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>17673941</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>17674275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>17674538</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>17674742</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>17675168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>17709692</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>20318360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>21525807</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>21609304</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>21759033</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>22329765</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>22632813</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>23172891</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>25678815</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>25681287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>25681842</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25788063</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25788195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27185621</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27187919</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>27189348</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30492632</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31628016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32444332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32574755</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>32574862</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>32713837</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>32714357</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>32714560</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>33014623</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>33318157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>33633249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>33761599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>34570722</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>35371856</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>36025478</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>38500081</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>42314885</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>44548104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>44548253</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>44548362</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>44548571</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>44761159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>44761313</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>44761943</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>44762073</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>44762812</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>44762872</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>45284831</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>45285576</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>45285716</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>53848289</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>55195364</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>57670530</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>57673764</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>59799165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>59799169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>59799172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>59799173</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>59799174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>59799176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>59799179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>59799182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>59799183</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>59799184</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>59799185</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>59799186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>59799187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>59799188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>59799189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>59799194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>59799195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>59799196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>59799197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>59799199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>59799202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>61555271</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>61618658</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>61638258</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>61638981</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>61639387</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>61639693</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>62574059</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>62574984</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>62594239</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>62594745</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>63872085</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>63875583</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>63894157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>64012864</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>64148805</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>64150702</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>64159247</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>64172970</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>64689891</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>64693659</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>64714388</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>65254062</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>65376456</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>65377173</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>65377754</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>66199641</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>66200420</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>66348448</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>66960526</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="6">
+        <v>93529418</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>32714266</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>17673603</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>17674610</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>74129864</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>20926636</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>33286629</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>33014374</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>59799200</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>73722730</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>91208613</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>7436160</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>74636752</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>74674306</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>74692933</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>74693837</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>74797507</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>78368732</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>91574130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>91573648</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>78367681</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>78352402</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>78350389</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>83303211</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>91572503</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>89401725</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>91573366</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>88795966</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>88756488</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>75848413</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>93025781</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>90163433</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>90145651</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>90163071</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>96709571</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>96726928</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>96766445</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>96657184</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="7">
+        <v>964664519</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>96770291</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>96768021</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>96523361</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>96380683</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>96360396</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>96192425</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>96171382</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>96170198</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>96080887</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>96063900</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>96149397</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>96006630</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>95953224</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>96081660</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>96082340</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>96808610</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>95715308</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>95752285</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>95690458</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>95796436</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>95539331</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>95434856</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>95410786</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>95341472</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>95337847</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>95749514</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>95722601</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>95205390</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>95123440</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>95162249</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>94936831</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>94939963</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>95056805</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>94767465</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>94796128</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>94666214</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>94322088</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>94235352</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>94210286</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>93846931</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>93845351</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>93836678</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>93827715</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>93709677</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>93696084</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>93671343</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>93669198</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>93510815</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>93503280</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>93459737</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>93476341</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>93443596</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>93445293</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>93393651</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>93237842</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>93234753</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>93233755</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>93232306</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>93214906</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>93214068</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>93201798</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>92890307</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>93025781</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>93021829</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>94731393</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>91741433</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" s="7">
+        <v>91105247</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>91056329</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>91104487</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>90847770</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>99519259</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>99310529</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>99324533</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>96170198</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>96171382</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>95796436</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>95056805</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>96722498</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>99280982</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>95162249</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>97209531</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>96063900</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>96080887</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>96726928</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>96808610</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>96464519</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>96523361</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>96380683</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>96192425</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>96657184</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>94936831</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>96360396</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>95752285</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>95715308</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>96006630</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" s="7">
+        <v>99794311</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>96932681</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>